<commit_message>
missing manual tests results
</commit_message>
<xml_diff>
--- a/test results/2013-01-07/Manualtests.xlsx
+++ b/test results/2013-01-07/Manualtests.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenwe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenwe\git\MuTicTacToe\test results\2013-01-07\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8475" windowHeight="6600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="4">
   <si>
     <t>Test number</t>
   </si>
@@ -269,10 +269,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -925,16 +925,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1209675</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1219,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,12 +1253,12 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <f>COUNTIFS($B$2:$B$58, D$1)</f>
-        <v>21</v>
+        <f>COUNTIFS($B$2:$B$153, D$1)</f>
+        <v>112</v>
       </c>
       <c r="E2">
-        <f>COUNTIFS($B$2:$B$58, E$1)</f>
-        <v>36</v>
+        <f>COUNTIFS($B$2:$B$153, E$1)</f>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1298,7 +1298,7 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1538,7 +1538,7 @@
         <v>307</v>
       </c>
       <c r="B37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1554,7 +1554,7 @@
         <v>309</v>
       </c>
       <c r="B39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1562,7 +1562,7 @@
         <v>310</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1570,7 +1570,7 @@
         <v>311</v>
       </c>
       <c r="B41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1578,7 +1578,7 @@
         <v>312</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1586,7 +1586,7 @@
         <v>313</v>
       </c>
       <c r="B43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1650,7 +1650,7 @@
         <v>321</v>
       </c>
       <c r="B51" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1658,7 +1658,7 @@
         <v>322</v>
       </c>
       <c r="B52" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1666,7 +1666,7 @@
         <v>323</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1674,7 +1674,7 @@
         <v>324</v>
       </c>
       <c r="B54" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1682,7 +1682,7 @@
         <v>325</v>
       </c>
       <c r="B55" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1690,7 +1690,7 @@
         <v>326</v>
       </c>
       <c r="B56" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1698,7 +1698,7 @@
         <v>327</v>
       </c>
       <c r="B57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1706,7 +1706,767 @@
         <v>328</v>
       </c>
       <c r="B58" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>329</v>
+      </c>
+      <c r="B59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>330</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>401</v>
+      </c>
+      <c r="B61" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>402</v>
+      </c>
+      <c r="B62" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>403</v>
+      </c>
+      <c r="B63" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>404</v>
+      </c>
+      <c r="B64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>405</v>
+      </c>
+      <c r="B65" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>406</v>
+      </c>
+      <c r="B66" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>407</v>
+      </c>
+      <c r="B67" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>408</v>
+      </c>
+      <c r="B68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>409</v>
+      </c>
+      <c r="B69" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>410</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>411</v>
+      </c>
+      <c r="B71" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>412</v>
+      </c>
+      <c r="B72" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>413</v>
+      </c>
+      <c r="B73" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>414</v>
+      </c>
+      <c r="B74" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>415</v>
+      </c>
+      <c r="B75" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>416</v>
+      </c>
+      <c r="B76" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>417</v>
+      </c>
+      <c r="B77" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>418</v>
+      </c>
+      <c r="B78" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>419</v>
+      </c>
+      <c r="B79" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>420</v>
+      </c>
+      <c r="B80" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>421</v>
+      </c>
+      <c r="B81" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>422</v>
+      </c>
+      <c r="B82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>423</v>
+      </c>
+      <c r="B83" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>424</v>
+      </c>
+      <c r="B84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>425</v>
+      </c>
+      <c r="B85" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>426</v>
+      </c>
+      <c r="B86" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>427</v>
+      </c>
+      <c r="B87" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>428</v>
+      </c>
+      <c r="B88" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>429</v>
+      </c>
+      <c r="B89" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>430</v>
+      </c>
+      <c r="B90" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>431</v>
+      </c>
+      <c r="B91" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>432</v>
+      </c>
+      <c r="B92" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>433</v>
+      </c>
+      <c r="B93" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>434</v>
+      </c>
+      <c r="B94" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>435</v>
+      </c>
+      <c r="B95" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>436</v>
+      </c>
+      <c r="B96" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>437</v>
+      </c>
+      <c r="B97" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>438</v>
+      </c>
+      <c r="B98" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>439</v>
+      </c>
+      <c r="B99" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>440</v>
+      </c>
+      <c r="B100" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>441</v>
+      </c>
+      <c r="B101" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>442</v>
+      </c>
+      <c r="B102" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>443</v>
+      </c>
+      <c r="B103" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>444</v>
+      </c>
+      <c r="B104" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>445</v>
+      </c>
+      <c r="B105" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>446</v>
+      </c>
+      <c r="B106" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>447</v>
+      </c>
+      <c r="B107" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>448</v>
+      </c>
+      <c r="B108" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>449</v>
+      </c>
+      <c r="B109" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>450</v>
+      </c>
+      <c r="B110" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>451</v>
+      </c>
+      <c r="B111" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>452</v>
+      </c>
+      <c r="B112" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>453</v>
+      </c>
+      <c r="B113" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>454</v>
+      </c>
+      <c r="B114" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>455</v>
+      </c>
+      <c r="B115" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>456</v>
+      </c>
+      <c r="B116" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>457</v>
+      </c>
+      <c r="B117" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>458</v>
+      </c>
+      <c r="B118" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>459</v>
+      </c>
+      <c r="B119" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>460</v>
+      </c>
+      <c r="B120" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>461</v>
+      </c>
+      <c r="B121" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>462</v>
+      </c>
+      <c r="B122" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>463</v>
+      </c>
+      <c r="B123" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>464</v>
+      </c>
+      <c r="B124" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>465</v>
+      </c>
+      <c r="B125" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>466</v>
+      </c>
+      <c r="B126" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>467</v>
+      </c>
+      <c r="B127" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>468</v>
+      </c>
+      <c r="B128" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>469</v>
+      </c>
+      <c r="B129" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>470</v>
+      </c>
+      <c r="B130" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>471</v>
+      </c>
+      <c r="B131" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>472</v>
+      </c>
+      <c r="B132" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>473</v>
+      </c>
+      <c r="B133" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>474</v>
+      </c>
+      <c r="B134" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>501</v>
+      </c>
+      <c r="B135" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>502</v>
+      </c>
+      <c r="B136" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>503</v>
+      </c>
+      <c r="B137" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>504</v>
+      </c>
+      <c r="B138" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>505</v>
+      </c>
+      <c r="B139" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>506</v>
+      </c>
+      <c r="B140" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>507</v>
+      </c>
+      <c r="B141" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>508</v>
+      </c>
+      <c r="B142" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>509</v>
+      </c>
+      <c r="B143" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>510</v>
+      </c>
+      <c r="B144" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>511</v>
+      </c>
+      <c r="B145" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>512</v>
+      </c>
+      <c r="B146" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>513</v>
+      </c>
+      <c r="B147" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>514</v>
+      </c>
+      <c r="B148" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>515</v>
+      </c>
+      <c r="B149" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>516</v>
+      </c>
+      <c r="B150" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>517</v>
+      </c>
+      <c r="B151" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>518</v>
+      </c>
+      <c r="B152" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>519</v>
+      </c>
+      <c r="B153" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>